<commit_message>
finish notes for 2021-12-16
</commit_message>
<xml_diff>
--- a/academic/Eaton_et_al._2021_Plague_in_Denmark_1000-1800.xlsx
+++ b/academic/Eaton_et_al._2021_Plague_in_Denmark_1000-1800.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktmea\Projects\obsidian-public\academic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291470E7-1DF2-4641-A3E7-DBB929A21395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524085BB-C35D-40AA-9B6D-E92BDFFEDE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="1430" windowWidth="21660" windowHeight="10590" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="3" r:id="rId1"/>
@@ -414,7 +414,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5104" uniqueCount="923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5105" uniqueCount="924">
   <si>
     <t>Cemetery</t>
   </si>
@@ -3174,31 +3174,55 @@
     <t>--</t>
   </si>
   <si>
-    <t>Total Individuals</t>
-  </si>
-  <si>
     <t>Plague Positive %</t>
   </si>
   <si>
-    <t>Individuals Sampled for Mitochondrial Analysis</t>
-  </si>
-  <si>
     <t>Full Mito Individuals</t>
   </si>
   <si>
-    <t>Human Positive %</t>
-  </si>
-  <si>
     <t>Negative</t>
   </si>
   <si>
-    <t>1350-1650</t>
-  </si>
-  <si>
     <t>1650-1800</t>
   </si>
   <si>
-    <t>1000-1350</t>
+    <t>Individuals</t>
+  </si>
+  <si>
+    <t>1000-1300</t>
+  </si>
+  <si>
+    <t>1300-1650</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Individuals Sampled for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Yersinia pestis</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Analysis</t>
+    </r>
+  </si>
+  <si>
+    <t>Individuals Sampled for Human Mitochondrial Analysis</t>
+  </si>
+  <si>
+    <t>Mito %</t>
   </si>
 </sst>
 </file>
@@ -3207,9 +3231,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3267,6 +3291,13 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -3481,7 +3512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3625,16 +3656,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3643,7 +3671,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4045,9 +4073,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMG322"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A225" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N323" sqref="N323"/>
+    <sheetView topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z315" sqref="Z315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7643,7 +7671,7 @@
       <c r="T63" s="51" t="s">
         <v>913</v>
       </c>
-      <c r="U63" s="69" t="s">
+      <c r="U63" s="68" t="s">
         <v>913</v>
       </c>
     </row>
@@ -7817,7 +7845,7 @@
       <c r="T66" s="51" t="s">
         <v>913</v>
       </c>
-      <c r="U66" s="69" t="s">
+      <c r="U66" s="68" t="s">
         <v>913</v>
       </c>
     </row>
@@ -8734,8 +8762,8 @@
       <c r="Q82" s="2"/>
       <c r="R82" s="22"/>
       <c r="S82" s="23"/>
-      <c r="T82" s="68"/>
-      <c r="U82" s="68"/>
+      <c r="T82" s="67"/>
+      <c r="U82" s="67"/>
     </row>
     <row r="83" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
@@ -9631,10 +9659,10 @@
       </c>
       <c r="Q98" s="2"/>
       <c r="R98" s="21"/>
-      <c r="T98" s="69" t="s">
+      <c r="T98" s="68" t="s">
         <v>913</v>
       </c>
-      <c r="U98" s="69" t="s">
+      <c r="U98" s="68" t="s">
         <v>913</v>
       </c>
     </row>
@@ -17926,10 +17954,10 @@
       </c>
       <c r="Q244" s="2"/>
       <c r="R244" s="33"/>
-      <c r="T244" s="69" t="s">
+      <c r="T244" s="68" t="s">
         <v>913</v>
       </c>
-      <c r="U244" s="69" t="s">
+      <c r="U244" s="68" t="s">
         <v>913</v>
       </c>
     </row>
@@ -18044,7 +18072,7 @@
       <c r="R246" s="33">
         <v>1</v>
       </c>
-      <c r="T246" s="69" t="s">
+      <c r="T246" s="68" t="s">
         <v>913</v>
       </c>
       <c r="U246" s="53" t="s">
@@ -20438,10 +20466,10 @@
       </c>
       <c r="Q288" s="2"/>
       <c r="R288" s="35"/>
-      <c r="T288" s="69" t="s">
+      <c r="T288" s="68" t="s">
         <v>913</v>
       </c>
-      <c r="U288" s="69" t="s">
+      <c r="U288" s="68" t="s">
         <v>913</v>
       </c>
     </row>
@@ -20554,10 +20582,10 @@
       </c>
       <c r="Q290" s="2"/>
       <c r="R290" s="35"/>
-      <c r="T290" s="69" t="s">
+      <c r="T290" s="68" t="s">
         <v>913</v>
       </c>
-      <c r="U290" s="69" t="s">
+      <c r="U290" s="68" t="s">
         <v>913</v>
       </c>
     </row>
@@ -20612,10 +20640,10 @@
       </c>
       <c r="Q291" s="2"/>
       <c r="R291" s="35"/>
-      <c r="T291" s="69" t="s">
+      <c r="T291" s="68" t="s">
         <v>913</v>
       </c>
-      <c r="U291" s="69" t="s">
+      <c r="U291" s="68" t="s">
         <v>913</v>
       </c>
     </row>
@@ -20728,10 +20756,10 @@
       </c>
       <c r="Q293" s="2"/>
       <c r="R293" s="35"/>
-      <c r="T293" s="69" t="s">
+      <c r="T293" s="68" t="s">
         <v>913</v>
       </c>
-      <c r="U293" s="69" t="s">
+      <c r="U293" s="68" t="s">
         <v>913</v>
       </c>
     </row>
@@ -20786,10 +20814,10 @@
       </c>
       <c r="Q294" s="2"/>
       <c r="R294" s="35"/>
-      <c r="T294" s="69" t="s">
+      <c r="T294" s="68" t="s">
         <v>913</v>
       </c>
-      <c r="U294" s="69" t="s">
+      <c r="U294" s="68" t="s">
         <v>913</v>
       </c>
     </row>
@@ -20960,10 +20988,10 @@
       </c>
       <c r="Q297" s="2"/>
       <c r="R297" s="35"/>
-      <c r="T297" s="69" t="s">
+      <c r="T297" s="68" t="s">
         <v>913</v>
       </c>
-      <c r="U297" s="69" t="s">
+      <c r="U297" s="68" t="s">
         <v>913</v>
       </c>
     </row>
@@ -21018,10 +21046,10 @@
       </c>
       <c r="Q298" s="2"/>
       <c r="R298" s="35"/>
-      <c r="T298" s="69" t="s">
+      <c r="T298" s="68" t="s">
         <v>913</v>
       </c>
-      <c r="U298" s="69" t="s">
+      <c r="U298" s="68" t="s">
         <v>913</v>
       </c>
     </row>
@@ -21296,7 +21324,7 @@
         <v>92</v>
       </c>
       <c r="N303" s="31"/>
-      <c r="O303" s="67" t="s">
+      <c r="O303" s="66" t="s">
         <v>527</v>
       </c>
       <c r="P303" s="3" t="s">
@@ -21364,7 +21392,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -21379,40 +21407,40 @@
     <col min="8" max="16384" width="8.7265625" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="52" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:7" ht="65" x14ac:dyDescent="0.3">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="61" t="s">
+        <v>921</v>
+      </c>
+      <c r="C1" s="61" t="s">
+        <v>799</v>
+      </c>
+      <c r="D1" s="61" t="s">
         <v>914</v>
       </c>
-      <c r="C1" s="62" t="s">
-        <v>799</v>
-      </c>
-      <c r="D1" s="62" t="s">
+      <c r="E1" s="61" t="s">
+        <v>922</v>
+      </c>
+      <c r="F1" s="61" t="s">
         <v>915</v>
       </c>
-      <c r="E1" s="62" t="s">
-        <v>916</v>
-      </c>
-      <c r="F1" s="62" t="s">
-        <v>917</v>
-      </c>
-      <c r="G1" s="62" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="G1" s="61" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
         <v>375</v>
       </c>
-      <c r="B2" s="58">
+      <c r="B2" s="57">
         <v>50</v>
       </c>
-      <c r="C2" s="58">
+      <c r="C2" s="57">
         <v>5</v>
       </c>
-      <c r="D2" s="63">
+      <c r="D2" s="62">
         <f>C2/B2</f>
         <v>0.1</v>
       </c>
@@ -21422,22 +21450,22 @@
       <c r="F2" s="57">
         <v>22</v>
       </c>
-      <c r="G2" s="64">
+      <c r="G2" s="63">
         <f>F2/E2</f>
         <v>0.5641025641025641</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="58">
+      <c r="B3" s="57">
         <v>17</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="57">
         <v>2</v>
       </c>
-      <c r="D3" s="63">
+      <c r="D3" s="62">
         <f t="shared" ref="D3:G9" si="0">C3/B3</f>
         <v>0.11764705882352941</v>
       </c>
@@ -21447,22 +21475,22 @@
       <c r="F3" s="55">
         <v>9</v>
       </c>
-      <c r="G3" s="64">
+      <c r="G3" s="63">
         <f t="shared" ref="G3:G8" si="1">F3/E3</f>
         <v>0.52941176470588236</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="58">
+      <c r="B4" s="57">
         <v>17</v>
       </c>
-      <c r="C4" s="58">
+      <c r="C4" s="57">
         <v>2</v>
       </c>
-      <c r="D4" s="63">
+      <c r="D4" s="62">
         <f t="shared" si="0"/>
         <v>0.11764705882352941</v>
       </c>
@@ -21472,22 +21500,22 @@
       <c r="F4" s="55">
         <v>5</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="63">
         <f t="shared" si="1"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="58">
+      <c r="B5" s="57">
         <v>25</v>
       </c>
-      <c r="C5" s="58">
+      <c r="C5" s="57">
         <v>1</v>
       </c>
-      <c r="D5" s="63">
+      <c r="D5" s="62">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
@@ -21497,22 +21525,22 @@
       <c r="F5" s="55">
         <v>6</v>
       </c>
-      <c r="G5" s="64">
+      <c r="G5" s="63">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B6" s="57">
         <v>11</v>
       </c>
-      <c r="C6" s="58">
+      <c r="C6" s="57">
         <v>1</v>
       </c>
-      <c r="D6" s="63">
+      <c r="D6" s="62">
         <f t="shared" si="0"/>
         <v>9.0909090909090912E-2</v>
       </c>
@@ -21522,22 +21550,22 @@
       <c r="F6" s="55">
         <v>7</v>
       </c>
-      <c r="G6" s="64">
+      <c r="G6" s="63">
         <f t="shared" si="1"/>
         <v>0.63636363636363635</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="58">
+      <c r="B7" s="57">
         <v>7</v>
       </c>
-      <c r="C7" s="58">
+      <c r="C7" s="57">
         <v>1</v>
       </c>
-      <c r="D7" s="63">
+      <c r="D7" s="62">
         <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
@@ -21547,102 +21575,107 @@
       <c r="F7" s="55">
         <v>3</v>
       </c>
-      <c r="G7" s="64">
+      <c r="G7" s="63">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="60" t="s">
         <v>712</v>
       </c>
-      <c r="B8" s="61">
+      <c r="B8" s="60">
         <v>28</v>
       </c>
-      <c r="C8" s="61">
+      <c r="C8" s="60">
         <v>1</v>
       </c>
-      <c r="D8" s="60">
+      <c r="D8" s="59">
         <f t="shared" si="0"/>
         <v>3.5714285714285712E-2</v>
       </c>
-      <c r="E8" s="59">
+      <c r="E8" s="58">
         <v>28</v>
       </c>
-      <c r="F8" s="59">
+      <c r="F8" s="58">
         <v>18</v>
       </c>
-      <c r="G8" s="66">
+      <c r="G8" s="65">
         <f t="shared" si="1"/>
         <v>0.6428571428571429</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="59">
+      <c r="B9" s="58">
         <f>SUM(B2:B8)</f>
         <v>155</v>
       </c>
-      <c r="C9" s="59">
+      <c r="C9" s="58">
         <f>SUM(C2:C8)</f>
         <v>13</v>
       </c>
-      <c r="D9" s="60">
+      <c r="D9" s="59">
         <f t="shared" si="0"/>
         <v>8.387096774193549E-2</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="58">
         <f>SUM(E2:E8)</f>
         <v>138</v>
       </c>
-      <c r="F9" s="59">
+      <c r="F9" s="58">
         <f>SUM(F2:F8)</f>
         <v>70</v>
       </c>
-      <c r="G9" s="60">
+      <c r="G9" s="59">
         <f t="shared" si="0"/>
         <v>0.50724637681159424</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA905D0D-FFAD-45C6-BD27-1881FA442351}">
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.08984375" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>918</v>
+      </c>
+      <c r="C2" t="s">
         <v>100</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>919</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>920</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
     </row>
   </sheetData>
@@ -21651,9 +21684,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21822,19 +21858,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2842305F-B6CA-4070-976E-7301810681B7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{242DC7CB-C41F-4F4F-AAF7-7469F922C91B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -21859,9 +21891,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{242DC7CB-C41F-4F4F-AAF7-7469F922C91B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2842305F-B6CA-4070-976E-7301810681B7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>